<commit_message>
changes working on the modbus, new known names file
</commit_message>
<xml_diff>
--- a/Panel Creator/KnownNames.xlsx
+++ b/Panel Creator/KnownNames.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Outside Air Temp</t>
   </si>
@@ -87,18 +87,6 @@
     <t>Variable Name</t>
   </si>
   <si>
-    <t>Name A</t>
-  </si>
-  <si>
-    <t>Name B</t>
-  </si>
-  <si>
-    <t>Name C</t>
-  </si>
-  <si>
-    <t>Name D</t>
-  </si>
-  <si>
     <t>~RackA\SGr1\SP Measure</t>
   </si>
   <si>
@@ -163,6 +151,66 @@
   </si>
   <si>
     <t>Suction Temp -28 Rack A</t>
+  </si>
+  <si>
+    <t>`%rackname` `%sgname` `%compname` Run Measure</t>
+  </si>
+  <si>
+    <t>Formatted Name</t>
+  </si>
+  <si>
+    <t>`%rackname` `%sgname` `%compname` SLA Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` Cnd `%fannum` Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` Cnd COP Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` Cnd DLT Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` Cnd COP2COT Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` Cnd CtrlStPt Command</t>
+  </si>
+  <si>
+    <t>`%rackname` `%sgname` DpTripPt Command</t>
+  </si>
+  <si>
+    <t>Discharge Temp `%rackname`</t>
+  </si>
+  <si>
+    <t>Subcool `%rackname` Cond Subcooling Measure</t>
+  </si>
+  <si>
+    <t>Subcool `%rackname` LQT Out - Subcooler 1 Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` `%sysname` EEPR % Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` `%sgname` SP Measure</t>
+  </si>
+  <si>
+    <t>`%rackname` `%sgname` SpStPt Measure</t>
+  </si>
+  <si>
+    <t>Suction Temp `%sgname` `%rackname`</t>
+  </si>
+  <si>
+    <t>Known Name 1</t>
+  </si>
+  <si>
+    <t>Known Name 2</t>
+  </si>
+  <si>
+    <t>Known Name 3</t>
+  </si>
+  <si>
+    <t>Known Name 4</t>
   </si>
 </sst>
 </file>
@@ -517,277 +565,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A2:A23"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.140625" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="9"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="9"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="9"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="9"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="1"/>
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="9"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="9"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="1"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:E99">
     <sortCondition ref="A2:A99"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed save/load for display size
</commit_message>
<xml_diff>
--- a/Panel Creator/KnownNames.xlsx
+++ b/Panel Creator/KnownNames.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="360" yWindow="135" windowWidth="16275" windowHeight="7485"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Points" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>Outside Air Temp</t>
   </si>
@@ -156,9 +155,6 @@
     <t>`%rackname` `%sgname` `%compname` Run Measure</t>
   </si>
   <si>
-    <t>Formatted Name</t>
-  </si>
-  <si>
     <t>`%rackname` `%sgname` `%compname` SLA Measure</t>
   </si>
   <si>
@@ -201,16 +197,43 @@
     <t>Suction Temp `%sgname` `%rackname`</t>
   </si>
   <si>
-    <t>Known Name 1</t>
-  </si>
-  <si>
-    <t>Known Name 2</t>
-  </si>
-  <si>
-    <t>Known Name 3</t>
-  </si>
-  <si>
-    <t>Known Name 4</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>sensor</t>
+  </si>
+  <si>
+    <t>FN 1</t>
+  </si>
+  <si>
+    <t>KN 1</t>
+  </si>
+  <si>
+    <t>FN 2</t>
+  </si>
+  <si>
+    <t>KN 2</t>
+  </si>
+  <si>
+    <t>FN 3</t>
+  </si>
+  <si>
+    <t>KN 3</t>
+  </si>
+  <si>
+    <t>FN 4</t>
+  </si>
+  <si>
+    <t>KN 4</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>TC SG1 SLA cmp1 A Measure</t>
+  </si>
+  <si>
+    <t>TC SG1 Run cmp1 A Measure</t>
   </si>
 </sst>
 </file>
@@ -252,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -264,6 +287,12 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,327 +594,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="C20" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="9"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="9"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="9"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="9"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="9"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="9"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="9"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
-      <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
-      <c r="C40" s="9"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="9"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="9"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" s="9"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="9"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="4"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62" s="1"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="1"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" s="1"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="1"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="9"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="9"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="9"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="4"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="1"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="1"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="1"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:E99">
@@ -894,28 +956,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>